<commit_message>
Create Bulk Upload Excel for subject-types and subject-categories and subjects and Plan and PlanSubject in web and API
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/plans.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/plans.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4B6551-57D0-498C-9238-3823FC6B1C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55CEFAB-8AB2-4E64-BAE0-7447F6570085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>plan_id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>كالوريوس هندسة نظم الحاسوب</t>
-  </si>
-  <si>
     <t>دبلوم التركيبات الكهربائية</t>
   </si>
   <si>
@@ -61,6 +58,33 @@
   </si>
   <si>
     <t>دبلوم التحكم الصناعي</t>
+  </si>
+  <si>
+    <t>بكالوريوس هندسة نظم الحاسوب</t>
+  </si>
+  <si>
+    <t>يعمري انتا ما احلاك</t>
+  </si>
+  <si>
+    <t>دبلوم محاسبة</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>العلوم الإدارية والمالية</t>
+  </si>
+  <si>
+    <t>department_id</t>
+  </si>
+  <si>
+    <t>إعلام رقمي</t>
+  </si>
+  <si>
+    <t>اعلام رقمي</t>
+  </si>
+  <si>
+    <t>العلوم التطبيقية</t>
   </si>
 </sst>
 </file>
@@ -102,9 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="عادي" xfId="0" builtinId="0"/>
@@ -385,20 +412,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.25" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,18 +443,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>2020</v>
@@ -437,16 +468,19 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>2020</v>
@@ -457,16 +491,19 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>333</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>2020</v>
@@ -477,16 +514,19 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>2020</v>
@@ -495,18 +535,21 @@
         <v>72</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>555</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>2020</v>
@@ -515,18 +558,21 @@
         <v>73</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>666</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>2020</v>
@@ -535,10 +581,142 @@
         <v>73</v>
       </c>
       <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>777</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2020</v>
+      </c>
+      <c r="E9">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>888</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>2020</v>
+      </c>
+      <c r="E10">
+        <v>73</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>2020</v>
+      </c>
+      <c r="E12">
+        <v>73</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>2020</v>
+      </c>
+      <c r="E13">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>666</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>2020</v>
+      </c>
+      <c r="E14">
+        <v>73</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:F11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>